<commit_message>
add file with mapping of variable names to product attribute descriptions
</commit_message>
<xml_diff>
--- a/post-analysis/code/attributes.xlsx
+++ b/post-analysis/code/attributes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanne\Dropbox\Tilburg\Projects\GfK Singapore\shared\Code\post-analysis\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATTA\Dropbox\Tilburg\Projects\GfK Singapore\shared\Code\post-analysis\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB70C53-C854-4765-AEBF-8B74AF21D3F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="114">
   <si>
     <t>category</t>
   </si>
@@ -229,12 +228,6 @@
     <t>Megapixels</t>
   </si>
   <si>
-    <t>Digital zoom available (indicator)</t>
-  </si>
-  <si>
-    <t>Blueray available (indicator)</t>
-  </si>
-  <si>
     <t>RAM (in MB)</t>
   </si>
   <si>
@@ -244,9 +237,6 @@
     <t>Hard disk size</t>
   </si>
   <si>
-    <t>without LEDs (indicator)</t>
-  </si>
-  <si>
     <t>Weight (in kg)</t>
   </si>
   <si>
@@ -256,12 +246,6 @@
     <t>Power (in watt)</t>
   </si>
   <si>
-    <t>With digital time controller (indicator)</t>
-  </si>
-  <si>
-    <t>Freezer available (indicator)</t>
-  </si>
-  <si>
     <t>Number of doors</t>
   </si>
   <si>
@@ -274,42 +258,6 @@
     <t>gsub</t>
   </si>
   <si>
-    <t>Screensize: &lt; 40 inch (indicator; baseline unknown screensizes)</t>
-  </si>
-  <si>
-    <t>Screensize: &gt;= 40 inch (indicator; baseline unknown screensizes)</t>
-  </si>
-  <si>
-    <t>Screensize: &lt;= 24 inch (indicator; baseline: others)</t>
-  </si>
-  <si>
-    <t>Screensize: &gt; 24 inch (indicator; baseline &gt; 24 inch)</t>
-  </si>
-  <si>
-    <t>Recording function (indicator)</t>
-  </si>
-  <si>
-    <t>3D available (indicator)</t>
-  </si>
-  <si>
-    <t>Touchscreen available (indicator)</t>
-  </si>
-  <si>
-    <t>Webcam available (indicator)</t>
-  </si>
-  <si>
-    <t>Microwave only (e.g,. without grill) (indicator)</t>
-  </si>
-  <si>
-    <t>Wifi available (indicator)</t>
-  </si>
-  <si>
-    <t>Bluetooth available (indicator)</t>
-  </si>
-  <si>
-    <t>Screensize: &lt;40 inch (indicator; baseline unknown screensizes)</t>
-  </si>
-  <si>
     <t>attr[_]screensize[_]recodesmeqth24inch</t>
   </si>
   <si>
@@ -364,19 +312,67 @@
     <t>attr[_]typetop</t>
   </si>
   <si>
-    <t>Extra functionality (indicator; baseline: washing only)</t>
-  </si>
-  <si>
-    <t>Front loader (indicator; baseline is others)</t>
-  </si>
-  <si>
-    <t>Other type (indicator; baseline is others)</t>
+    <t>Screensize: Indicator variable, equaling 1 if screensize &lt;= 24 inch, 0 otherwise (baseline: unknown screensizes)</t>
+  </si>
+  <si>
+    <t>Screensize: Indicator variable, equaling 1 if screensize &gt; 24 inch, 0 otherwise (baseline: unknown screensizes)</t>
+  </si>
+  <si>
+    <t>Digital zoom: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Blueray: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Recording function: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>without LEDs: Indicator variable, equaling 1 for LCD TVs without LEDs, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Screensize: Indicator variable, equaling 1 if screensize &lt; 40 inch, 0 otherwise (baseline: unknown screensizes)</t>
+  </si>
+  <si>
+    <t>Screensize: Indicator variable, equaling 1 if screensize &gt;= 40 inch, 0 otherwise (baseline: unknown screensizes)</t>
+  </si>
+  <si>
+    <t>3D: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Touchscreen: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Webcam: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Functionality: Indicator variable, equaling 1 for only microwave functionality, 0 otherwise (e.g., if microwave comes with a grill)</t>
+  </si>
+  <si>
+    <t>Digital time controller: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Wifi: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Bluetooth: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Freezer: Indicator variable, equaling 1 if available, 0 otherwise</t>
+  </si>
+  <si>
+    <t>Functionality: Indicator variable, equaling 1 if washing machine comes with extra functionality; 0 if washing only</t>
+  </si>
+  <si>
+    <t>Top loader: Indicator variable, equaling 1 if top loader; 0 otherwise (baseline is others)</t>
+  </si>
+  <si>
+    <t>Front loader: Indicator variable, equaling 1 if front loader; 0 otherwise (baseline is others)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,12 +382,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -406,8 +408,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,19 +690,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -766,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -801,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -836,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -871,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -906,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -941,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -976,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1816,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2306,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2411,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2446,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2481,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2516,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2691,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2761,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2796,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2831,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2936,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2971,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3076,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3111,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3146,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3216,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3251,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3321,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3356,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3391,7 +3394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3496,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3531,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3601,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3636,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3671,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3706,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3776,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3846,7 +3849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3881,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3916,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3951,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4021,7 +4024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4056,7 +4059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4091,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4196,7 +4199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4231,7 +4234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4266,7 +4269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4336,7 +4339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4371,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4406,7 +4409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4441,7 +4444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4476,7 +4479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4511,7 +4514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4546,7 +4549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4581,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4616,7 +4619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4651,7 +4654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4686,7 +4689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4721,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4756,7 +4759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4791,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4826,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4931,7 +4934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4966,7 +4969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5001,7 +5004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5036,7 +5039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5071,7 +5074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5106,7 +5109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5141,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5176,7 +5179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5211,7 +5214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5246,7 +5249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5281,7 +5284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5316,7 +5319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5351,7 +5354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5386,7 +5389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5421,7 +5424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5456,7 +5459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5491,7 +5494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5526,7 +5529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5561,7 +5564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5631,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5666,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5701,7 +5704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5736,7 +5739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5771,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5806,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5841,7 +5844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5876,7 +5879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5911,7 +5914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5946,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5981,7 +5984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6051,7 +6054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6086,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6121,7 +6124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6156,7 +6159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6191,7 +6194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6226,7 +6229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6261,7 +6264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6296,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6331,7 +6334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6366,7 +6369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6401,7 +6404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6471,7 +6474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6506,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6541,7 +6544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6576,7 +6579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6611,7 +6614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6646,7 +6649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6681,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6716,7 +6719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6751,7 +6754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6786,7 +6789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6821,7 +6824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6856,7 +6859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6926,7 +6929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6961,7 +6964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6996,7 +6999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -7031,7 +7034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -7066,7 +7069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -7101,7 +7104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -7136,7 +7139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -7177,22 +7180,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -7203,718 +7206,718 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C12" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>49</v>
       </c>
-      <c r="C27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>50</v>
       </c>
-      <c r="C28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>50</v>
       </c>
-      <c r="C29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
       </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>51</v>
       </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>52</v>
       </c>
-      <c r="C33" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>52</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
       </c>
-      <c r="C35" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>52</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D36" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>53</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D39" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>54</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D40" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>54</v>
       </c>
-      <c r="C41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" t="s">
-        <v>112</v>
-      </c>
-      <c r="E41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
       </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
       </c>
-      <c r="C43" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" t="s">
-        <v>81</v>
+      <c r="C43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>